<commit_message>
Transaction download fix with cloudinary
</commit_message>
<xml_diff>
--- a/src/excel/FashionsTransactions.xlsx
+++ b/src/excel/FashionsTransactions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="222">
   <si>
     <t>ID</t>
   </si>
@@ -702,6 +702,25 @@
   </si>
   <si>
     <t>Gaun Pesta Elegan - Satin Coklat - One SIze</t>
+  </si>
+  <si>
+    <t>65d8144d9dcadcc6f33c77bd</t>
+  </si>
+  <si>
+    <t>2/23/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peci Brokat Muslim - Base - L
+Peci Brokat Muslim - Base - XL</t>
+  </si>
+  <si>
+    <t>Rp. 58,900</t>
+  </si>
+  <si>
+    <t>65ddfaa404ada948c61fa88e</t>
+  </si>
+  <si>
+    <t>2/27/2024</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1106,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I59"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="9" width="30" customWidth="1"/>
@@ -2746,6 +2765,64 @@
         <v>14</v>
       </c>
     </row>
+    <row r="58" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>